<commit_message>
Refactoring, added new .py code
</commit_message>
<xml_diff>
--- a/ExtractionResults/ExtractionResults.xlsx
+++ b/ExtractionResults/ExtractionResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DianaGradinaru\Documents\GitHub\SignatureDetection_TextractPython\ExtractionResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DianaGradinaru\Documents\GitHub\SignatureDetection_Textract\ExtractionResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A154E4-0492-459C-8258-AD0623620205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F793974-824F-4808-A0B4-56C7D943EC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="1304" windowWidth="23095" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>